<commit_message>
Update codes that Califications
</commit_message>
<xml_diff>
--- a/Cursos.xlsx
+++ b/Cursos.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galigaribaldi/Documents/PPropios/Validador_Py/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE9D955-1A4E-ED4A-A217-A649BEC573AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>ID_Curso</t>
   </si>
@@ -31,6 +25,36 @@
     <t>Descripcion</t>
   </si>
   <si>
+    <t>283913077412</t>
+  </si>
+  <si>
+    <t>126383120623</t>
+  </si>
+  <si>
+    <t>126382430066</t>
+  </si>
+  <si>
+    <t>126382430048</t>
+  </si>
+  <si>
+    <t>126382430032</t>
+  </si>
+  <si>
+    <t>126382430010</t>
+  </si>
+  <si>
+    <t>126382145238</t>
+  </si>
+  <si>
+    <t>126382145220</t>
+  </si>
+  <si>
+    <t>126380062908</t>
+  </si>
+  <si>
+    <t>126316206557</t>
+  </si>
+  <si>
     <t>291374157706</t>
   </si>
   <si>
@@ -61,6 +85,12 @@
     <t>Computación K3</t>
   </si>
   <si>
+    <t>Computación K2</t>
+  </si>
+  <si>
+    <t>Computación K1</t>
+  </si>
+  <si>
     <t>Curso Nuevo de Prueba</t>
   </si>
   <si>
@@ -89,6 +119,12 @@
   </si>
   <si>
     <t>Computación K3 Materia ExtraCurricular</t>
+  </si>
+  <si>
+    <t>Computación K2 Materia Extracurricular</t>
+  </si>
+  <si>
+    <t>Computación K1 Materia extracurricular</t>
   </si>
   <si>
     <t>Este es un curso de pruena</t>
@@ -100,8 +136,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,19 +200,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -218,7 +246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,27 +278,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -302,24 +312,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -495,21 +487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,144 +505,172 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>283913077412</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>126383120623</v>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>126382430066</v>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>126382430048</v>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>126382430032</v>
+      <c r="B6" t="s">
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>126382430010</v>
+      <c r="B7" t="s">
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>126382145238</v>
+      <c r="B8" t="s">
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>126382145220</v>
+      <c r="B9" t="s">
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
-        <v>24</v>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>